<commit_message>
Added backend to get sample measurements of simulation
</commit_message>
<xml_diff>
--- a/media/experiment spreadsheets/Experiment.xlsx
+++ b/media/experiment spreadsheets/Experiment.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10411"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10509"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/niklasgrenningloh/Documents/EWV/media/experiment spreadsheets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FBFC95B-B5D0-4E47-9337-48E2B7BBFF02}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62B884D3-DC3F-814C-A612-CA1466651C70}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16480" xr2:uid="{CE282B59-617A-B644-A507-1F04EC4F5DBB}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191028"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="17">
   <si>
     <t>U in V</t>
   </si>
@@ -66,17 +66,32 @@
     <t>Angaben in mm</t>
   </si>
   <si>
-    <t>U in V2</t>
+    <t>Y=6,3</t>
   </si>
   <si>
-    <t>Zu Großmaschig (ungenauigkeit)</t>
+    <t>Y=12,6</t>
+  </si>
+  <si>
+    <t>Hallo ich bin ZZ</t>
+  </si>
+  <si>
+    <t>Zu Großmaschig (Ungenauigkeit)</t>
+  </si>
+  <si>
+    <t>s von der Aluminumplatte</t>
+  </si>
+  <si>
+    <t>Spalte1</t>
+  </si>
+  <si>
+    <t>Vermutung für neue werte ist der Winkel der Platte</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -98,16 +113,28 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor theme="4" tint="0.79998168889431442"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -115,14 +142,29 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </right>
+      <top style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </top>
+      <bottom style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -210,10 +252,10 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Tabelle1!$J$9:$J$39</c:f>
+              <c:f>Tabelle1!$J$9:$J$54</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="31"/>
+                <c:ptCount val="46"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
@@ -306,16 +348,61 @@
                 </c:pt>
                 <c:pt idx="30">
                   <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>31</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>33</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>34</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>35</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>36</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>37</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>38</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>39</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>41</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>42</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>43</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>44</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>45</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Tabelle1!$K$9:$K$39</c:f>
+              <c:f>Tabelle1!$K$9:$K$54</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="31"/>
+                <c:ptCount val="46"/>
                 <c:pt idx="0">
                   <c:v>0.23</c:v>
                 </c:pt>
@@ -350,16 +437,64 @@
                   <c:v>0.3</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.28000000000000003</c:v>
+                  <c:v>0.28999999999999998</c:v>
                 </c:pt>
                 <c:pt idx="12">
                   <c:v>0.26</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0.24</c:v>
+                  <c:v>0.23</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>0.21</c:v>
+                  <c:v>0.19</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.15</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.09</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.04</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.02</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0.06</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>0.13</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>0.22</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>0.25</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>0.28999999999999998</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>0.31</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>0.31</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>0.28999999999999998</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>0.26</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>0.23</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>0.2</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>0.16</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -380,7 +515,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>U in V2</c:v>
+                  <c:v>Spalte1</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -411,10 +546,10 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Tabelle1!$J$9:$J$39</c:f>
+              <c:f>Tabelle1!$J$9:$J$54</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="31"/>
+                <c:ptCount val="46"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
@@ -507,78 +642,90 @@
                 </c:pt>
                 <c:pt idx="30">
                   <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>31</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>33</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>34</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>35</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>36</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>37</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>38</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>39</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>41</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>42</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>43</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>44</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>45</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Tabelle1!$L$9:$L$39</c:f>
+              <c:f>Tabelle1!$L$9:$L$54</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="31"/>
-                <c:pt idx="10">
-                  <c:v>0.3</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>0.28999999999999998</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>0.26</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>0.23</c:v>
-                </c:pt>
-                <c:pt idx="14">
+                <c:ptCount val="46"/>
+                <c:pt idx="31">
+                  <c:v>0.08</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>0.02</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>0.02</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>0.1</c:v>
+                </c:pt>
+                <c:pt idx="35">
                   <c:v>0.19</c:v>
                 </c:pt>
-                <c:pt idx="15">
-                  <c:v>0.15</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>0.09</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>0.04</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>0.02</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>0.06</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>0.13</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>0.22</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>0.25</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>0.28999999999999998</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>0.31</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>0.31</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>0.28999999999999998</c:v>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v>0.26</c:v>
-                </c:pt>
-                <c:pt idx="28">
-                  <c:v>0.23</c:v>
-                </c:pt>
-                <c:pt idx="29">
-                  <c:v>0.2</c:v>
-                </c:pt>
-                <c:pt idx="30">
-                  <c:v>0.16</c:v>
+                <c:pt idx="36">
+                  <c:v>0.32</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>0.39</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>0.41</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>0.38</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>0.35</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -586,7 +733,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000003-254E-0D4B-A2F2-07C1A2D60849}"/>
+              <c16:uniqueId val="{00000003-FF73-9A47-A897-F9B0B46888B8}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1330,16 +1477,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>400050</xdr:colOff>
-      <xdr:row>6</xdr:row>
-      <xdr:rowOff>57150</xdr:rowOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>628650</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>69850</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>18</xdr:col>
-      <xdr:colOff>19050</xdr:colOff>
-      <xdr:row>19</xdr:row>
-      <xdr:rowOff>158750</xdr:rowOff>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1368,12 +1515,12 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{8E43C0ED-5288-6D44-8413-DCE226FDE2BE}" name="Tabelle1" displayName="Tabelle1" ref="J8:L39" totalsRowShown="0">
-  <autoFilter ref="J8:L39" xr:uid="{4BA24919-8958-5140-9DA1-FB888B3D7714}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{8E43C0ED-5288-6D44-8413-DCE226FDE2BE}" name="Tabelle1" displayName="Tabelle1" ref="J8:L54" totalsRowShown="0">
+  <autoFilter ref="J8:L54" xr:uid="{4BA24919-8958-5140-9DA1-FB888B3D7714}"/>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{FFA2FA7B-E8F1-8A4D-903D-E4B859890653}" name="s in mm "/>
-    <tableColumn id="2" xr3:uid="{39E4DC6D-B2AC-A441-A7E5-A31224D72601}" name="U in V"/>
-    <tableColumn id="3" xr3:uid="{8C671E23-0B7B-924E-9BED-6E2C0E540457}" name="U in V2"/>
+    <tableColumn id="3" xr3:uid="{8C671E23-0B7B-924E-9BED-6E2C0E540457}" name="U in V"/>
+    <tableColumn id="2" xr3:uid="{2D8C8A5F-6613-7C46-9DC1-AAED0365AAD9}" name="Spalte1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1402,8 +1549,8 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{35481FE6-2EF6-DB42-82BE-DA31979F4FA6}" name="Tabelle4" displayName="Tabelle4" ref="T6:U12" totalsRowShown="0">
-  <autoFilter ref="T6:U12" xr:uid="{18207B99-3524-854A-B295-81FD2EDFEBDA}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{35481FE6-2EF6-DB42-82BE-DA31979F4FA6}" name="Tabelle4" displayName="Tabelle4" ref="U6:V12" totalsRowShown="0">
+  <autoFilter ref="U6:V12" xr:uid="{18207B99-3524-854A-B295-81FD2EDFEBDA}"/>
   <tableColumns count="2">
     <tableColumn id="1" xr3:uid="{DC45F120-F1AC-F04D-82EE-26B71BB18B13}" name="Minima "/>
     <tableColumn id="2" xr3:uid="{BE8AC687-9FBD-124D-8174-56A416BFCAEB}" name="Maxima"/>
@@ -1709,15 +1856,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AF7205EF-FC57-874B-9099-CF57BA48A150}">
-  <dimension ref="A3:U39"/>
+  <dimension ref="A3:ZZ54"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P24" sqref="P24"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="Q20" sqref="Q20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:702" x14ac:dyDescent="0.2">
       <c r="B3" t="s">
         <v>5</v>
       </c>
@@ -1725,34 +1872,40 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:702" x14ac:dyDescent="0.2">
       <c r="D4" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="T4" t="s">
+      <c r="U4" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="6" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="ZZ4" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" spans="1:702" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="F6" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="T6" t="s">
+      <c r="U6" t="s">
         <v>3</v>
       </c>
-      <c r="U6" t="s">
+      <c r="V6" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="T7">
+    <row r="7" spans="1:702" x14ac:dyDescent="0.2">
+      <c r="J7" t="s">
+        <v>14</v>
+      </c>
+      <c r="U7">
         <v>3.7</v>
       </c>
     </row>
-    <row r="8" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:702" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>1</v>
       </c>
@@ -1772,13 +1925,13 @@
         <v>0</v>
       </c>
       <c r="L8" t="s">
+        <v>15</v>
+      </c>
+      <c r="V8">
         <v>10</v>
       </c>
-      <c r="U8">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="9" spans="1:21" x14ac:dyDescent="0.2">
+    </row>
+    <row r="9" spans="1:702" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>0</v>
       </c>
@@ -1797,11 +1950,11 @@
       <c r="K9">
         <v>0.23</v>
       </c>
-      <c r="T9">
+      <c r="U9">
         <v>17.899999999999999</v>
       </c>
     </row>
-    <row r="10" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:702" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>0.5</v>
       </c>
@@ -1820,11 +1973,11 @@
       <c r="K10">
         <v>0.2</v>
       </c>
-      <c r="U10">
+      <c r="V10">
         <v>24.5</v>
       </c>
     </row>
-    <row r="11" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:702" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>1</v>
       </c>
@@ -1843,11 +1996,11 @@
       <c r="K11">
         <v>0.16</v>
       </c>
-      <c r="T11">
+      <c r="U11">
         <v>32.5</v>
       </c>
     </row>
-    <row r="12" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:702" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>1.5</v>
       </c>
@@ -1866,11 +2019,11 @@
       <c r="K12">
         <v>0.09</v>
       </c>
-      <c r="U12">
+      <c r="V12">
         <v>38</v>
       </c>
     </row>
-    <row r="13" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:702" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>2</v>
       </c>
@@ -1890,7 +2043,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="14" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:702" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>2.5</v>
       </c>
@@ -1909,8 +2062,14 @@
       <c r="K14">
         <v>0.04</v>
       </c>
-    </row>
-    <row r="15" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="U14" t="s">
+        <v>10</v>
+      </c>
+      <c r="V14" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="15" spans="1:702" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>3</v>
       </c>
@@ -1924,7 +2083,7 @@
         <v>0.13</v>
       </c>
     </row>
-    <row r="16" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:702" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>3.5</v>
       </c>
@@ -1938,7 +2097,7 @@
         <v>0.18</v>
       </c>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>4</v>
       </c>
@@ -1952,7 +2111,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>4.5</v>
       </c>
@@ -1966,7 +2125,7 @@
         <v>0.28999999999999998</v>
       </c>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>5</v>
       </c>
@@ -1979,11 +2138,8 @@
       <c r="K19">
         <v>0.3</v>
       </c>
-      <c r="L19">
-        <v>0.3</v>
-      </c>
-    </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.2">
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>5.5</v>
       </c>
@@ -1994,13 +2150,10 @@
         <v>11</v>
       </c>
       <c r="K20">
-        <v>0.28000000000000003</v>
-      </c>
-      <c r="L20">
         <v>0.28999999999999998</v>
       </c>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>6</v>
       </c>
@@ -2013,11 +2166,8 @@
       <c r="K21">
         <v>0.26</v>
       </c>
-      <c r="L21">
-        <v>0.26</v>
-      </c>
-    </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.2">
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>6.5</v>
       </c>
@@ -2028,13 +2178,10 @@
         <v>13</v>
       </c>
       <c r="K22">
-        <v>0.24</v>
-      </c>
-      <c r="L22">
         <v>0.23</v>
       </c>
     </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>7</v>
       </c>
@@ -2045,13 +2192,10 @@
         <v>14</v>
       </c>
       <c r="K23">
-        <v>0.21</v>
-      </c>
-      <c r="L23">
         <v>0.19</v>
       </c>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>7.5</v>
       </c>
@@ -2061,11 +2205,11 @@
       <c r="J24">
         <v>15</v>
       </c>
-      <c r="L24">
+      <c r="K24">
         <v>0.15</v>
       </c>
     </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>8</v>
       </c>
@@ -2075,11 +2219,11 @@
       <c r="J25">
         <v>16</v>
       </c>
-      <c r="L25">
+      <c r="K25">
         <v>0.09</v>
       </c>
     </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>8.5</v>
       </c>
@@ -2089,115 +2233,240 @@
       <c r="J26">
         <v>17</v>
       </c>
-      <c r="L26">
+      <c r="K26">
         <v>0.04</v>
       </c>
     </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.2">
       <c r="J27">
         <v>18</v>
       </c>
-      <c r="L27">
+      <c r="K27">
         <v>0.02</v>
       </c>
     </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.2">
       <c r="J28">
         <v>19</v>
       </c>
-      <c r="L28">
+      <c r="K28">
         <v>0.06</v>
       </c>
     </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.2">
       <c r="J29">
         <v>20</v>
       </c>
-      <c r="L29">
+      <c r="K29">
         <v>0.13</v>
       </c>
     </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.2">
       <c r="J30">
         <v>21</v>
       </c>
-      <c r="L30">
+      <c r="K30">
         <v>0.22</v>
       </c>
     </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.2">
       <c r="J31">
         <v>22</v>
       </c>
-      <c r="L31">
+      <c r="K31">
         <v>0.25</v>
       </c>
     </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.2">
       <c r="J32">
         <v>23</v>
       </c>
-      <c r="L32">
+      <c r="K32">
         <v>0.28999999999999998</v>
       </c>
     </row>
-    <row r="33" spans="10:12" x14ac:dyDescent="0.2">
+    <row r="33" spans="8:14" x14ac:dyDescent="0.2">
       <c r="J33">
         <v>24</v>
       </c>
-      <c r="L33">
+      <c r="K33">
         <v>0.31</v>
       </c>
     </row>
-    <row r="34" spans="10:12" x14ac:dyDescent="0.2">
+    <row r="34" spans="8:14" x14ac:dyDescent="0.2">
       <c r="J34">
         <v>25</v>
       </c>
-      <c r="L34">
+      <c r="K34">
         <v>0.31</v>
       </c>
     </row>
-    <row r="35" spans="10:12" x14ac:dyDescent="0.2">
+    <row r="35" spans="8:14" x14ac:dyDescent="0.2">
+      <c r="H35" s="4"/>
       <c r="J35">
         <v>26</v>
       </c>
-      <c r="L35">
+      <c r="K35">
         <v>0.28999999999999998</v>
       </c>
     </row>
-    <row r="36" spans="10:12" x14ac:dyDescent="0.2">
+    <row r="36" spans="8:14" x14ac:dyDescent="0.2">
+      <c r="H36" s="3"/>
       <c r="J36">
         <v>27</v>
       </c>
-      <c r="L36">
+      <c r="K36">
         <v>0.26</v>
       </c>
     </row>
-    <row r="37" spans="10:12" x14ac:dyDescent="0.2">
+    <row r="37" spans="8:14" x14ac:dyDescent="0.2">
+      <c r="H37" s="4"/>
       <c r="J37">
         <v>28</v>
       </c>
-      <c r="L37">
+      <c r="K37">
         <v>0.23</v>
       </c>
     </row>
-    <row r="38" spans="10:12" x14ac:dyDescent="0.2">
+    <row r="38" spans="8:14" x14ac:dyDescent="0.2">
+      <c r="H38" s="3"/>
       <c r="J38">
         <v>29</v>
       </c>
-      <c r="L38">
+      <c r="K38">
         <v>0.2</v>
       </c>
     </row>
-    <row r="39" spans="10:12" x14ac:dyDescent="0.2">
+    <row r="39" spans="8:14" x14ac:dyDescent="0.2">
+      <c r="H39" s="4"/>
       <c r="J39">
         <v>30</v>
       </c>
-      <c r="L39">
+      <c r="K39">
         <v>0.16</v>
       </c>
     </row>
+    <row r="40" spans="8:14" x14ac:dyDescent="0.2">
+      <c r="H40" s="3"/>
+      <c r="J40" s="1">
+        <v>31</v>
+      </c>
+      <c r="L40" s="1">
+        <v>0.08</v>
+      </c>
+      <c r="N40" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="41" spans="8:14" x14ac:dyDescent="0.2">
+      <c r="H41" s="4"/>
+      <c r="J41">
+        <v>32</v>
+      </c>
+      <c r="L41" s="1">
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="42" spans="8:14" x14ac:dyDescent="0.2">
+      <c r="H42" s="3"/>
+      <c r="J42">
+        <v>33</v>
+      </c>
+      <c r="L42" s="1">
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="43" spans="8:14" x14ac:dyDescent="0.2">
+      <c r="H43" s="4"/>
+      <c r="J43">
+        <v>34</v>
+      </c>
+      <c r="L43" s="1">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="44" spans="8:14" x14ac:dyDescent="0.2">
+      <c r="H44" s="3"/>
+      <c r="J44">
+        <v>35</v>
+      </c>
+      <c r="L44" s="1">
+        <v>0.19</v>
+      </c>
+    </row>
+    <row r="45" spans="8:14" x14ac:dyDescent="0.2">
+      <c r="H45" s="4"/>
+      <c r="J45">
+        <v>36</v>
+      </c>
+      <c r="L45" s="1">
+        <v>0.32</v>
+      </c>
+    </row>
+    <row r="46" spans="8:14" x14ac:dyDescent="0.2">
+      <c r="H46" s="3"/>
+      <c r="J46">
+        <v>37</v>
+      </c>
+      <c r="L46" s="1">
+        <v>0.39</v>
+      </c>
+    </row>
+    <row r="47" spans="8:14" x14ac:dyDescent="0.2">
+      <c r="H47" s="4"/>
+      <c r="J47">
+        <v>38</v>
+      </c>
+      <c r="L47" s="1">
+        <v>0.41</v>
+      </c>
+    </row>
+    <row r="48" spans="8:14" x14ac:dyDescent="0.2">
+      <c r="H48" s="3"/>
+      <c r="J48">
+        <v>39</v>
+      </c>
+      <c r="L48" s="1">
+        <v>0.38</v>
+      </c>
+    </row>
+    <row r="49" spans="8:12" x14ac:dyDescent="0.2">
+      <c r="H49" s="4"/>
+      <c r="J49">
+        <v>40</v>
+      </c>
+      <c r="L49" s="1">
+        <v>0.35</v>
+      </c>
+    </row>
+    <row r="50" spans="8:12" x14ac:dyDescent="0.2">
+      <c r="H50" s="3"/>
+      <c r="J50">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="51" spans="8:12" x14ac:dyDescent="0.2">
+      <c r="J51">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="52" spans="8:12" x14ac:dyDescent="0.2">
+      <c r="J52">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="53" spans="8:12" x14ac:dyDescent="0.2">
+      <c r="J53">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="54" spans="8:12" x14ac:dyDescent="0.2">
+      <c r="J54">
+        <v>45</v>
+      </c>
+    </row>
   </sheetData>
+  <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
   <tableParts count="4">

</xml_diff>

<commit_message>
Changed formula, Changed variables and unnecessary variable conversions, Changed Settings UI, made new experiments
</commit_message>
<xml_diff>
--- a/media/experiment spreadsheets/Experiment.xlsx
+++ b/media/experiment spreadsheets/Experiment.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10509"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10808"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/niklasgrenningloh/Documents/EWV/media/experiment spreadsheets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62B884D3-DC3F-814C-A612-CA1466651C70}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F77D87B-8AD9-DF4A-B5DE-43D0B753B185}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16480" xr2:uid="{CE282B59-617A-B644-A507-1F04EC4F5DBB}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="26">
   <si>
     <t>U in V</t>
   </si>
@@ -85,6 +85,33 @@
   </si>
   <si>
     <t>Vermutung für neue werte ist der Winkel der Platte</t>
+  </si>
+  <si>
+    <t>Reihne 1</t>
+  </si>
+  <si>
+    <t>in ma</t>
+  </si>
+  <si>
+    <t>Spalte2</t>
+  </si>
+  <si>
+    <t>in µa</t>
+  </si>
+  <si>
+    <t>Spalte3</t>
+  </si>
+  <si>
+    <t>Spalte4</t>
+  </si>
+  <si>
+    <t>Abstand in mm</t>
+  </si>
+  <si>
+    <t>Spalte5</t>
+  </si>
+  <si>
+    <t>Durchschnitt</t>
   </si>
 </sst>
 </file>
@@ -159,17 +186,22 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="1">
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -734,6 +766,213 @@
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000003-FF73-9A47-A897-F9B0B46888B8}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Tabelle1!$M$8</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Reihne 1</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent3"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Tabelle1!$J$9:$J$54</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="46"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>19</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>21</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>23</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>26</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>27</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>28</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>29</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>31</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>33</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>34</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>35</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>36</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>37</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>38</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>39</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>41</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>42</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>43</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>44</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>45</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Tabelle1!$M$9:$M$54</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="46"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-7AF4-4C46-ACE2-88D06D8D6621}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -917,7 +1156,1390 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="de-DE"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="de-DE"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="2.5815965382822503E-2"/>
+          <c:y val="0.10739278325547545"/>
+          <c:w val="0.95339475474287194"/>
+          <c:h val="0.81548803454745034"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Tabelle1!$AC$7:$AC$68</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="62"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>19</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>19</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>21</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>21</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>5</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-87D0-AB4C-A757-9F50CE0EBEEC}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Tabelle1!$AD$7:$AD$68</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="62"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>19</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>21</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>21</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>6</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-87D0-AB4C-A757-9F50CE0EBEEC}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Tabelle1!$AE$7:$AE$68</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="62"/>
+                <c:pt idx="0">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>19</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>5</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-87D0-AB4C-A757-9F50CE0EBEEC}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Tabelle1!$AF$7:$AF$68</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="62"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>19</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>19</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>21</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>19</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>3</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-6CEA-DB4C-8CE0-1963BBD0EF65}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:v>Durchschnitt</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent5"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Tabelle1!$AG$7:$AG$68</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="62"/>
+                <c:pt idx="0">
+                  <c:v>1.25</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.25</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>10.75</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>15.5</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>16.25</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>13.75</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>11.25</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>7.25</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>1.25</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>4.25</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>17.75</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>1.25</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>2.75</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>8.5</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>13.75</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>19.5</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>18.75</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>13.5</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>4.25</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>1.75</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>0.75</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>0.25</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>1.25</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>4.5</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>9.25</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>16.5</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>20.75</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>20.25</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>10.75</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>2.75</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>4.75</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-6CEA-DB4C-8CE0-1963BBD0EF65}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="492519264"/>
+        <c:axId val="492424880"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="492519264"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="de-DE"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="492424880"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="492424880"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="de-DE"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="492519264"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="de-DE"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="de-DE"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.78740157499999996" l="0.7" r="0.7" t="0.78740157499999996" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
   <a:schemeClr val="accent2"/>
@@ -1473,20 +3095,536 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>628650</xdr:colOff>
-      <xdr:row>4</xdr:row>
-      <xdr:rowOff>69850</xdr:rowOff>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>679450</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>44450</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>18</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>17</xdr:row>
-      <xdr:rowOff>171450</xdr:rowOff>
+      <xdr:col>26</xdr:col>
+      <xdr:colOff>50800</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>146050</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1511,16 +3649,53 @@
     </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>39</xdr:col>
+      <xdr:colOff>139516</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>55405</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>50</xdr:col>
+      <xdr:colOff>636331</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>44715</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Diagramm 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{47E0BDA6-E70B-A347-ADD9-DB81D8E88BBF}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{8E43C0ED-5288-6D44-8413-DCE226FDE2BE}" name="Tabelle1" displayName="Tabelle1" ref="J8:L54" totalsRowShown="0">
-  <autoFilter ref="J8:L54" xr:uid="{4BA24919-8958-5140-9DA1-FB888B3D7714}"/>
-  <tableColumns count="3">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{8E43C0ED-5288-6D44-8413-DCE226FDE2BE}" name="Tabelle1" displayName="Tabelle1" ref="J8:M54" totalsRowShown="0">
+  <autoFilter ref="J8:M54" xr:uid="{4BA24919-8958-5140-9DA1-FB888B3D7714}"/>
+  <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{FFA2FA7B-E8F1-8A4D-903D-E4B859890653}" name="s in mm "/>
     <tableColumn id="3" xr3:uid="{8C671E23-0B7B-924E-9BED-6E2C0E540457}" name="U in V"/>
     <tableColumn id="2" xr3:uid="{2D8C8A5F-6613-7C46-9DC1-AAED0365AAD9}" name="Spalte1"/>
+    <tableColumn id="4" xr3:uid="{407FF294-693D-0E4A-9395-6206CA72C38F}" name="Reihne 1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1554,6 +3729,23 @@
   <tableColumns count="2">
     <tableColumn id="1" xr3:uid="{DC45F120-F1AC-F04D-82EE-26B71BB18B13}" name="Minima "/>
     <tableColumn id="2" xr3:uid="{BE8AC687-9FBD-124D-8174-56A416BFCAEB}" name="Maxima"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{8A10AC3B-6965-0244-A36B-E8576B22127E}" name="Tabelle5" displayName="Tabelle5" ref="AB6:AG68" totalsRowShown="0">
+  <autoFilter ref="AB6:AG68" xr:uid="{8A10AC3B-6965-0244-A36B-E8576B22127E}"/>
+  <tableColumns count="6">
+    <tableColumn id="1" xr3:uid="{56674A68-4091-A548-9B8E-76BC4B47F87C}" name="Abstand in mm"/>
+    <tableColumn id="2" xr3:uid="{DD3D4A4A-FCC4-8649-AE63-45FB366BB9B7}" name="Spalte2"/>
+    <tableColumn id="3" xr3:uid="{336A243E-43E1-E24E-972A-50BCA977BFB4}" name="Spalte3"/>
+    <tableColumn id="4" xr3:uid="{5C40AE0B-5C17-0749-BFEC-AE7CD1449C2B}" name="Spalte4"/>
+    <tableColumn id="5" xr3:uid="{4F9A44CE-C914-2643-BEC0-669AA5DDCB8C}" name="Spalte5"/>
+    <tableColumn id="6" xr3:uid="{5A8968D7-26ED-CF44-8679-635D6517759D}" name="Durchschnitt" dataDxfId="0">
+      <calculatedColumnFormula>(Tabelle5[[#This Row],[Spalte2]]+Tabelle5[[#This Row],[Spalte3]]+Tabelle5[[#This Row],[Spalte4]]+Tabelle5[[#This Row],[Spalte5]])/4</calculatedColumnFormula>
+    </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1856,10 +4048,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AF7205EF-FC57-874B-9099-CF57BA48A150}">
-  <dimension ref="A3:ZZ54"/>
+  <dimension ref="A3:ZZ68"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="Q20" sqref="Q20"/>
+    <sheetView tabSelected="1" topLeftCell="AN6" zoomScale="159" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="BA15" sqref="BA15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1879,8 +4071,25 @@
       <c r="U4" t="s">
         <v>9</v>
       </c>
+      <c r="AC4" s="5">
+        <v>44449</v>
+      </c>
+      <c r="AD4" s="5">
+        <v>44449</v>
+      </c>
+      <c r="AE4" s="5">
+        <v>44449</v>
+      </c>
+      <c r="AF4" s="5">
+        <v>44470</v>
+      </c>
       <c r="ZZ4" t="s">
         <v>12</v>
+      </c>
+    </row>
+    <row r="5" spans="1:702" x14ac:dyDescent="0.2">
+      <c r="AC5" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="6" spans="1:702" x14ac:dyDescent="0.2">
@@ -1896,13 +4105,53 @@
       <c r="V6" t="s">
         <v>4</v>
       </c>
+      <c r="AB6" t="s">
+        <v>23</v>
+      </c>
+      <c r="AC6" t="s">
+        <v>19</v>
+      </c>
+      <c r="AD6" t="s">
+        <v>21</v>
+      </c>
+      <c r="AE6" t="s">
+        <v>22</v>
+      </c>
+      <c r="AF6" t="s">
+        <v>24</v>
+      </c>
+      <c r="AG6" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="7" spans="1:702" x14ac:dyDescent="0.2">
       <c r="J7" t="s">
         <v>14</v>
       </c>
+      <c r="M7" t="s">
+        <v>18</v>
+      </c>
       <c r="U7">
         <v>3.7</v>
+      </c>
+      <c r="AB7">
+        <v>0</v>
+      </c>
+      <c r="AC7">
+        <v>1</v>
+      </c>
+      <c r="AD7">
+        <v>1</v>
+      </c>
+      <c r="AE7">
+        <v>2</v>
+      </c>
+      <c r="AF7">
+        <v>1</v>
+      </c>
+      <c r="AG7">
+        <f>(Tabelle5[[#This Row],[Spalte2]]+Tabelle5[[#This Row],[Spalte3]]+Tabelle5[[#This Row],[Spalte4]]+Tabelle5[[#This Row],[Spalte5]])/4</f>
+        <v>1.25</v>
       </c>
     </row>
     <row r="8" spans="1:702" x14ac:dyDescent="0.2">
@@ -1927,9 +4176,31 @@
       <c r="L8" t="s">
         <v>15</v>
       </c>
+      <c r="M8" t="s">
+        <v>17</v>
+      </c>
       <c r="V8">
         <v>10</v>
       </c>
+      <c r="AB8">
+        <v>1</v>
+      </c>
+      <c r="AC8">
+        <v>0</v>
+      </c>
+      <c r="AD8">
+        <v>0</v>
+      </c>
+      <c r="AE8">
+        <v>0</v>
+      </c>
+      <c r="AF8">
+        <v>0</v>
+      </c>
+      <c r="AG8">
+        <f>(Tabelle5[[#This Row],[Spalte2]]+Tabelle5[[#This Row],[Spalte3]]+Tabelle5[[#This Row],[Spalte4]]+Tabelle5[[#This Row],[Spalte5]])/4</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="9" spans="1:702" x14ac:dyDescent="0.2">
       <c r="A9">
@@ -1950,8 +4221,30 @@
       <c r="K9">
         <v>0.23</v>
       </c>
+      <c r="M9">
+        <v>0</v>
+      </c>
       <c r="U9">
         <v>17.899999999999999</v>
+      </c>
+      <c r="AB9">
+        <v>2</v>
+      </c>
+      <c r="AC9">
+        <v>0</v>
+      </c>
+      <c r="AD9">
+        <v>0</v>
+      </c>
+      <c r="AE9">
+        <v>0</v>
+      </c>
+      <c r="AF9">
+        <v>0</v>
+      </c>
+      <c r="AG9">
+        <f>(Tabelle5[[#This Row],[Spalte2]]+Tabelle5[[#This Row],[Spalte3]]+Tabelle5[[#This Row],[Spalte4]]+Tabelle5[[#This Row],[Spalte5]])/4</f>
+        <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:702" x14ac:dyDescent="0.2">
@@ -1976,6 +4269,25 @@
       <c r="V10">
         <v>24.5</v>
       </c>
+      <c r="AB10">
+        <v>3</v>
+      </c>
+      <c r="AC10">
+        <v>0</v>
+      </c>
+      <c r="AD10">
+        <v>0</v>
+      </c>
+      <c r="AE10">
+        <v>0</v>
+      </c>
+      <c r="AF10">
+        <v>0</v>
+      </c>
+      <c r="AG10">
+        <f>(Tabelle5[[#This Row],[Spalte2]]+Tabelle5[[#This Row],[Spalte3]]+Tabelle5[[#This Row],[Spalte4]]+Tabelle5[[#This Row],[Spalte5]])/4</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="11" spans="1:702" x14ac:dyDescent="0.2">
       <c r="A11">
@@ -1996,8 +4308,30 @@
       <c r="K11">
         <v>0.16</v>
       </c>
+      <c r="M11">
+        <v>0</v>
+      </c>
       <c r="U11">
         <v>32.5</v>
+      </c>
+      <c r="AB11">
+        <v>4</v>
+      </c>
+      <c r="AC11">
+        <v>1</v>
+      </c>
+      <c r="AD11">
+        <v>2</v>
+      </c>
+      <c r="AE11">
+        <v>1</v>
+      </c>
+      <c r="AF11">
+        <v>1</v>
+      </c>
+      <c r="AG11">
+        <f>(Tabelle5[[#This Row],[Spalte2]]+Tabelle5[[#This Row],[Spalte3]]+Tabelle5[[#This Row],[Spalte4]]+Tabelle5[[#This Row],[Spalte5]])/4</f>
+        <v>1.25</v>
       </c>
     </row>
     <row r="12" spans="1:702" x14ac:dyDescent="0.2">
@@ -2022,6 +4356,25 @@
       <c r="V12">
         <v>38</v>
       </c>
+      <c r="AB12">
+        <v>5</v>
+      </c>
+      <c r="AC12">
+        <v>6</v>
+      </c>
+      <c r="AD12">
+        <v>5</v>
+      </c>
+      <c r="AE12">
+        <v>3</v>
+      </c>
+      <c r="AF12">
+        <v>2</v>
+      </c>
+      <c r="AG12">
+        <f>(Tabelle5[[#This Row],[Spalte2]]+Tabelle5[[#This Row],[Spalte3]]+Tabelle5[[#This Row],[Spalte4]]+Tabelle5[[#This Row],[Spalte5]])/4</f>
+        <v>4</v>
+      </c>
     </row>
     <row r="13" spans="1:702" x14ac:dyDescent="0.2">
       <c r="A13">
@@ -2042,6 +4395,25 @@
       <c r="K13">
         <v>0.02</v>
       </c>
+      <c r="AB13">
+        <v>6</v>
+      </c>
+      <c r="AC13">
+        <v>9</v>
+      </c>
+      <c r="AD13">
+        <v>12</v>
+      </c>
+      <c r="AE13">
+        <v>13</v>
+      </c>
+      <c r="AF13">
+        <v>9</v>
+      </c>
+      <c r="AG13">
+        <f>(Tabelle5[[#This Row],[Spalte2]]+Tabelle5[[#This Row],[Spalte3]]+Tabelle5[[#This Row],[Spalte4]]+Tabelle5[[#This Row],[Spalte5]])/4</f>
+        <v>10.75</v>
+      </c>
     </row>
     <row r="14" spans="1:702" x14ac:dyDescent="0.2">
       <c r="A14">
@@ -2068,6 +4440,25 @@
       <c r="V14" t="s">
         <v>11</v>
       </c>
+      <c r="AB14">
+        <v>7</v>
+      </c>
+      <c r="AC14">
+        <v>14</v>
+      </c>
+      <c r="AD14">
+        <v>16</v>
+      </c>
+      <c r="AE14">
+        <v>16</v>
+      </c>
+      <c r="AF14">
+        <v>16</v>
+      </c>
+      <c r="AG14">
+        <f>(Tabelle5[[#This Row],[Spalte2]]+Tabelle5[[#This Row],[Spalte3]]+Tabelle5[[#This Row],[Spalte4]]+Tabelle5[[#This Row],[Spalte5]])/4</f>
+        <v>15.5</v>
+      </c>
     </row>
     <row r="15" spans="1:702" x14ac:dyDescent="0.2">
       <c r="A15">
@@ -2082,6 +4473,25 @@
       <c r="K15">
         <v>0.13</v>
       </c>
+      <c r="AB15">
+        <v>8</v>
+      </c>
+      <c r="AC15">
+        <v>16</v>
+      </c>
+      <c r="AD15">
+        <v>16</v>
+      </c>
+      <c r="AE15">
+        <v>16</v>
+      </c>
+      <c r="AF15">
+        <v>17</v>
+      </c>
+      <c r="AG15">
+        <f>(Tabelle5[[#This Row],[Spalte2]]+Tabelle5[[#This Row],[Spalte3]]+Tabelle5[[#This Row],[Spalte4]]+Tabelle5[[#This Row],[Spalte5]])/4</f>
+        <v>16.25</v>
+      </c>
     </row>
     <row r="16" spans="1:702" x14ac:dyDescent="0.2">
       <c r="A16">
@@ -2096,8 +4506,27 @@
       <c r="K16">
         <v>0.18</v>
       </c>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="AB16">
+        <v>9</v>
+      </c>
+      <c r="AC16">
+        <v>14</v>
+      </c>
+      <c r="AD16">
+        <v>14</v>
+      </c>
+      <c r="AE16">
+        <v>14</v>
+      </c>
+      <c r="AF16">
+        <v>13</v>
+      </c>
+      <c r="AG16">
+        <f>(Tabelle5[[#This Row],[Spalte2]]+Tabelle5[[#This Row],[Spalte3]]+Tabelle5[[#This Row],[Spalte4]]+Tabelle5[[#This Row],[Spalte5]])/4</f>
+        <v>13.75</v>
+      </c>
+    </row>
+    <row r="17" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>4</v>
       </c>
@@ -2110,8 +4539,27 @@
       <c r="K17">
         <v>0.25</v>
       </c>
-    </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="AB17">
+        <v>10</v>
+      </c>
+      <c r="AC17">
+        <v>12</v>
+      </c>
+      <c r="AD17">
+        <v>13</v>
+      </c>
+      <c r="AE17">
+        <v>10</v>
+      </c>
+      <c r="AF17">
+        <v>10</v>
+      </c>
+      <c r="AG17">
+        <f>(Tabelle5[[#This Row],[Spalte2]]+Tabelle5[[#This Row],[Spalte3]]+Tabelle5[[#This Row],[Spalte4]]+Tabelle5[[#This Row],[Spalte5]])/4</f>
+        <v>11.25</v>
+      </c>
+    </row>
+    <row r="18" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>4.5</v>
       </c>
@@ -2124,8 +4572,27 @@
       <c r="K18">
         <v>0.28999999999999998</v>
       </c>
-    </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="AB18">
+        <v>11</v>
+      </c>
+      <c r="AC18">
+        <v>6</v>
+      </c>
+      <c r="AD18">
+        <v>9</v>
+      </c>
+      <c r="AE18">
+        <v>7</v>
+      </c>
+      <c r="AF18">
+        <v>7</v>
+      </c>
+      <c r="AG18">
+        <f>(Tabelle5[[#This Row],[Spalte2]]+Tabelle5[[#This Row],[Spalte3]]+Tabelle5[[#This Row],[Spalte4]]+Tabelle5[[#This Row],[Spalte5]])/4</f>
+        <v>7.25</v>
+      </c>
+    </row>
+    <row r="19" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>5</v>
       </c>
@@ -2138,8 +4605,27 @@
       <c r="K19">
         <v>0.3</v>
       </c>
-    </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="AB19">
+        <v>12</v>
+      </c>
+      <c r="AC19">
+        <v>3</v>
+      </c>
+      <c r="AD19">
+        <v>4</v>
+      </c>
+      <c r="AE19">
+        <v>4</v>
+      </c>
+      <c r="AF19">
+        <v>5</v>
+      </c>
+      <c r="AG19">
+        <f>(Tabelle5[[#This Row],[Spalte2]]+Tabelle5[[#This Row],[Spalte3]]+Tabelle5[[#This Row],[Spalte4]]+Tabelle5[[#This Row],[Spalte5]])/4</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="20" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>5.5</v>
       </c>
@@ -2152,8 +4638,27 @@
       <c r="K20">
         <v>0.28999999999999998</v>
       </c>
-    </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="AB20">
+        <v>13</v>
+      </c>
+      <c r="AC20">
+        <v>2</v>
+      </c>
+      <c r="AD20">
+        <v>2</v>
+      </c>
+      <c r="AE20">
+        <v>2</v>
+      </c>
+      <c r="AF20">
+        <v>2</v>
+      </c>
+      <c r="AG20">
+        <f>(Tabelle5[[#This Row],[Spalte2]]+Tabelle5[[#This Row],[Spalte3]]+Tabelle5[[#This Row],[Spalte4]]+Tabelle5[[#This Row],[Spalte5]])/4</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>6</v>
       </c>
@@ -2166,8 +4671,27 @@
       <c r="K21">
         <v>0.26</v>
       </c>
-    </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="AB21">
+        <v>14</v>
+      </c>
+      <c r="AC21">
+        <v>0</v>
+      </c>
+      <c r="AD21">
+        <v>0</v>
+      </c>
+      <c r="AE21">
+        <v>0</v>
+      </c>
+      <c r="AF21">
+        <v>0</v>
+      </c>
+      <c r="AG21">
+        <f>(Tabelle5[[#This Row],[Spalte2]]+Tabelle5[[#This Row],[Spalte3]]+Tabelle5[[#This Row],[Spalte4]]+Tabelle5[[#This Row],[Spalte5]])/4</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>6.5</v>
       </c>
@@ -2180,8 +4704,27 @@
       <c r="K22">
         <v>0.23</v>
       </c>
-    </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="AB22">
+        <v>15</v>
+      </c>
+      <c r="AC22">
+        <v>0</v>
+      </c>
+      <c r="AD22">
+        <v>0</v>
+      </c>
+      <c r="AE22">
+        <v>0</v>
+      </c>
+      <c r="AF22">
+        <v>0</v>
+      </c>
+      <c r="AG22">
+        <f>(Tabelle5[[#This Row],[Spalte2]]+Tabelle5[[#This Row],[Spalte3]]+Tabelle5[[#This Row],[Spalte4]]+Tabelle5[[#This Row],[Spalte5]])/4</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>7</v>
       </c>
@@ -2194,8 +4737,27 @@
       <c r="K23">
         <v>0.19</v>
       </c>
-    </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="AB23">
+        <v>16</v>
+      </c>
+      <c r="AC23">
+        <v>0</v>
+      </c>
+      <c r="AD23">
+        <v>0</v>
+      </c>
+      <c r="AE23">
+        <v>0</v>
+      </c>
+      <c r="AF23">
+        <v>0</v>
+      </c>
+      <c r="AG23">
+        <f>(Tabelle5[[#This Row],[Spalte2]]+Tabelle5[[#This Row],[Spalte3]]+Tabelle5[[#This Row],[Spalte4]]+Tabelle5[[#This Row],[Spalte5]])/4</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>7.5</v>
       </c>
@@ -2208,8 +4770,27 @@
       <c r="K24">
         <v>0.15</v>
       </c>
-    </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="AB24">
+        <v>17</v>
+      </c>
+      <c r="AC24">
+        <v>0</v>
+      </c>
+      <c r="AD24">
+        <v>0</v>
+      </c>
+      <c r="AE24">
+        <v>0</v>
+      </c>
+      <c r="AF24">
+        <v>0</v>
+      </c>
+      <c r="AG24">
+        <f>(Tabelle5[[#This Row],[Spalte2]]+Tabelle5[[#This Row],[Spalte3]]+Tabelle5[[#This Row],[Spalte4]]+Tabelle5[[#This Row],[Spalte5]])/4</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>8</v>
       </c>
@@ -2222,8 +4803,27 @@
       <c r="K25">
         <v>0.09</v>
       </c>
-    </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="AB25">
+        <v>18</v>
+      </c>
+      <c r="AC25">
+        <v>2</v>
+      </c>
+      <c r="AD25">
+        <v>1</v>
+      </c>
+      <c r="AE25">
+        <v>1</v>
+      </c>
+      <c r="AF25">
+        <v>1</v>
+      </c>
+      <c r="AG25">
+        <f>(Tabelle5[[#This Row],[Spalte2]]+Tabelle5[[#This Row],[Spalte3]]+Tabelle5[[#This Row],[Spalte4]]+Tabelle5[[#This Row],[Spalte5]])/4</f>
+        <v>1.25</v>
+      </c>
+    </row>
+    <row r="26" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>8.5</v>
       </c>
@@ -2236,72 +4836,243 @@
       <c r="K26">
         <v>0.04</v>
       </c>
-    </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="AB26">
+        <v>19</v>
+      </c>
+      <c r="AC26">
+        <v>5</v>
+      </c>
+      <c r="AD26">
+        <v>4</v>
+      </c>
+      <c r="AE26">
+        <v>4</v>
+      </c>
+      <c r="AF26">
+        <v>4</v>
+      </c>
+      <c r="AG26">
+        <f>(Tabelle5[[#This Row],[Spalte2]]+Tabelle5[[#This Row],[Spalte3]]+Tabelle5[[#This Row],[Spalte4]]+Tabelle5[[#This Row],[Spalte5]])/4</f>
+        <v>4.25</v>
+      </c>
+    </row>
+    <row r="27" spans="1:33" x14ac:dyDescent="0.2">
       <c r="J27">
         <v>18</v>
       </c>
       <c r="K27">
         <v>0.02</v>
       </c>
-    </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="AB27">
+        <v>20</v>
+      </c>
+      <c r="AC27">
+        <v>12</v>
+      </c>
+      <c r="AD27">
+        <v>10</v>
+      </c>
+      <c r="AE27">
+        <v>10</v>
+      </c>
+      <c r="AF27">
+        <v>8</v>
+      </c>
+      <c r="AG27">
+        <f>(Tabelle5[[#This Row],[Spalte2]]+Tabelle5[[#This Row],[Spalte3]]+Tabelle5[[#This Row],[Spalte4]]+Tabelle5[[#This Row],[Spalte5]])/4</f>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="28" spans="1:33" x14ac:dyDescent="0.2">
       <c r="J28">
         <v>19</v>
       </c>
       <c r="K28">
         <v>0.06</v>
       </c>
-    </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="AB28">
+        <v>21</v>
+      </c>
+      <c r="AC28">
+        <v>16</v>
+      </c>
+      <c r="AD28">
+        <v>16</v>
+      </c>
+      <c r="AE28">
+        <v>16</v>
+      </c>
+      <c r="AF28">
+        <v>16</v>
+      </c>
+      <c r="AG28">
+        <f>(Tabelle5[[#This Row],[Spalte2]]+Tabelle5[[#This Row],[Spalte3]]+Tabelle5[[#This Row],[Spalte4]]+Tabelle5[[#This Row],[Spalte5]])/4</f>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="29" spans="1:33" x14ac:dyDescent="0.2">
       <c r="J29">
         <v>20</v>
       </c>
       <c r="K29">
         <v>0.13</v>
       </c>
-    </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="AB29">
+        <v>22</v>
+      </c>
+      <c r="AC29">
+        <v>18</v>
+      </c>
+      <c r="AD29">
+        <v>18</v>
+      </c>
+      <c r="AE29">
+        <v>18</v>
+      </c>
+      <c r="AF29">
+        <v>17</v>
+      </c>
+      <c r="AG29">
+        <f>(Tabelle5[[#This Row],[Spalte2]]+Tabelle5[[#This Row],[Spalte3]]+Tabelle5[[#This Row],[Spalte4]]+Tabelle5[[#This Row],[Spalte5]])/4</f>
+        <v>17.75</v>
+      </c>
+    </row>
+    <row r="30" spans="1:33" x14ac:dyDescent="0.2">
       <c r="J30">
         <v>21</v>
       </c>
       <c r="K30">
         <v>0.22</v>
       </c>
-    </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="AB30">
+        <v>23</v>
+      </c>
+      <c r="AC30">
+        <v>16</v>
+      </c>
+      <c r="AD30">
+        <v>16</v>
+      </c>
+      <c r="AE30">
+        <v>16</v>
+      </c>
+      <c r="AF30">
+        <v>16</v>
+      </c>
+      <c r="AG30">
+        <f>(Tabelle5[[#This Row],[Spalte2]]+Tabelle5[[#This Row],[Spalte3]]+Tabelle5[[#This Row],[Spalte4]]+Tabelle5[[#This Row],[Spalte5]])/4</f>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="31" spans="1:33" x14ac:dyDescent="0.2">
       <c r="J31">
         <v>22</v>
       </c>
       <c r="K31">
         <v>0.25</v>
       </c>
-    </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="AB31">
+        <v>24</v>
+      </c>
+      <c r="AC31">
+        <v>12</v>
+      </c>
+      <c r="AD31">
+        <v>12</v>
+      </c>
+      <c r="AE31">
+        <v>12</v>
+      </c>
+      <c r="AF31">
+        <v>12</v>
+      </c>
+      <c r="AG31">
+        <f>(Tabelle5[[#This Row],[Spalte2]]+Tabelle5[[#This Row],[Spalte3]]+Tabelle5[[#This Row],[Spalte4]]+Tabelle5[[#This Row],[Spalte5]])/4</f>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="32" spans="1:33" x14ac:dyDescent="0.2">
       <c r="J32">
         <v>23</v>
       </c>
       <c r="K32">
         <v>0.28999999999999998</v>
       </c>
-    </row>
-    <row r="33" spans="8:14" x14ac:dyDescent="0.2">
+      <c r="AB32">
+        <v>25</v>
+      </c>
+      <c r="AC32">
+        <v>9</v>
+      </c>
+      <c r="AD32">
+        <v>8</v>
+      </c>
+      <c r="AE32">
+        <v>7</v>
+      </c>
+      <c r="AF32">
+        <v>8</v>
+      </c>
+      <c r="AG32">
+        <f>(Tabelle5[[#This Row],[Spalte2]]+Tabelle5[[#This Row],[Spalte3]]+Tabelle5[[#This Row],[Spalte4]]+Tabelle5[[#This Row],[Spalte5]])/4</f>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="33" spans="8:33" x14ac:dyDescent="0.2">
       <c r="J33">
         <v>24</v>
       </c>
       <c r="K33">
         <v>0.31</v>
       </c>
-    </row>
-    <row r="34" spans="8:14" x14ac:dyDescent="0.2">
+      <c r="AB33">
+        <v>26</v>
+      </c>
+      <c r="AC33">
+        <v>4</v>
+      </c>
+      <c r="AD33">
+        <v>4</v>
+      </c>
+      <c r="AE33">
+        <v>4</v>
+      </c>
+      <c r="AF33">
+        <v>4</v>
+      </c>
+      <c r="AG33">
+        <f>(Tabelle5[[#This Row],[Spalte2]]+Tabelle5[[#This Row],[Spalte3]]+Tabelle5[[#This Row],[Spalte4]]+Tabelle5[[#This Row],[Spalte5]])/4</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="34" spans="8:33" x14ac:dyDescent="0.2">
       <c r="J34">
         <v>25</v>
       </c>
       <c r="K34">
         <v>0.31</v>
       </c>
-    </row>
-    <row r="35" spans="8:14" x14ac:dyDescent="0.2">
+      <c r="AB34">
+        <v>27</v>
+      </c>
+      <c r="AC34">
+        <v>2</v>
+      </c>
+      <c r="AD34">
+        <v>2</v>
+      </c>
+      <c r="AE34">
+        <v>2</v>
+      </c>
+      <c r="AF34">
+        <v>2</v>
+      </c>
+      <c r="AG34">
+        <f>(Tabelle5[[#This Row],[Spalte2]]+Tabelle5[[#This Row],[Spalte3]]+Tabelle5[[#This Row],[Spalte4]]+Tabelle5[[#This Row],[Spalte5]])/4</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="35" spans="8:33" x14ac:dyDescent="0.2">
       <c r="H35" s="4"/>
       <c r="J35">
         <v>26</v>
@@ -2309,8 +5080,27 @@
       <c r="K35">
         <v>0.28999999999999998</v>
       </c>
-    </row>
-    <row r="36" spans="8:14" x14ac:dyDescent="0.2">
+      <c r="AB35">
+        <v>28</v>
+      </c>
+      <c r="AC35">
+        <v>1</v>
+      </c>
+      <c r="AD35">
+        <v>1</v>
+      </c>
+      <c r="AE35">
+        <v>1</v>
+      </c>
+      <c r="AF35">
+        <v>1</v>
+      </c>
+      <c r="AG35">
+        <f>(Tabelle5[[#This Row],[Spalte2]]+Tabelle5[[#This Row],[Spalte3]]+Tabelle5[[#This Row],[Spalte4]]+Tabelle5[[#This Row],[Spalte5]])/4</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="8:33" x14ac:dyDescent="0.2">
       <c r="H36" s="3"/>
       <c r="J36">
         <v>27</v>
@@ -2318,8 +5108,27 @@
       <c r="K36">
         <v>0.26</v>
       </c>
-    </row>
-    <row r="37" spans="8:14" x14ac:dyDescent="0.2">
+      <c r="AB36">
+        <v>29</v>
+      </c>
+      <c r="AC36">
+        <v>0</v>
+      </c>
+      <c r="AD36">
+        <v>0</v>
+      </c>
+      <c r="AE36">
+        <v>0</v>
+      </c>
+      <c r="AF36">
+        <v>0</v>
+      </c>
+      <c r="AG36">
+        <f>(Tabelle5[[#This Row],[Spalte2]]+Tabelle5[[#This Row],[Spalte3]]+Tabelle5[[#This Row],[Spalte4]]+Tabelle5[[#This Row],[Spalte5]])/4</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="8:33" x14ac:dyDescent="0.2">
       <c r="H37" s="4"/>
       <c r="J37">
         <v>28</v>
@@ -2327,8 +5136,27 @@
       <c r="K37">
         <v>0.23</v>
       </c>
-    </row>
-    <row r="38" spans="8:14" x14ac:dyDescent="0.2">
+      <c r="AB37">
+        <v>30</v>
+      </c>
+      <c r="AC37">
+        <v>0</v>
+      </c>
+      <c r="AD37">
+        <v>0</v>
+      </c>
+      <c r="AE37">
+        <v>0</v>
+      </c>
+      <c r="AF37">
+        <v>0</v>
+      </c>
+      <c r="AG37">
+        <f>(Tabelle5[[#This Row],[Spalte2]]+Tabelle5[[#This Row],[Spalte3]]+Tabelle5[[#This Row],[Spalte4]]+Tabelle5[[#This Row],[Spalte5]])/4</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="8:33" x14ac:dyDescent="0.2">
       <c r="H38" s="3"/>
       <c r="J38">
         <v>29</v>
@@ -2336,8 +5164,27 @@
       <c r="K38">
         <v>0.2</v>
       </c>
-    </row>
-    <row r="39" spans="8:14" x14ac:dyDescent="0.2">
+      <c r="AB38">
+        <v>31</v>
+      </c>
+      <c r="AC38">
+        <v>0</v>
+      </c>
+      <c r="AD38">
+        <v>0</v>
+      </c>
+      <c r="AE38">
+        <v>0</v>
+      </c>
+      <c r="AF38">
+        <v>0</v>
+      </c>
+      <c r="AG38">
+        <f>(Tabelle5[[#This Row],[Spalte2]]+Tabelle5[[#This Row],[Spalte3]]+Tabelle5[[#This Row],[Spalte4]]+Tabelle5[[#This Row],[Spalte5]])/4</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="8:33" x14ac:dyDescent="0.2">
       <c r="H39" s="4"/>
       <c r="J39">
         <v>30</v>
@@ -2345,8 +5192,27 @@
       <c r="K39">
         <v>0.16</v>
       </c>
-    </row>
-    <row r="40" spans="8:14" x14ac:dyDescent="0.2">
+      <c r="AB39">
+        <v>32</v>
+      </c>
+      <c r="AC39">
+        <v>1</v>
+      </c>
+      <c r="AD39">
+        <v>1</v>
+      </c>
+      <c r="AE39">
+        <v>2</v>
+      </c>
+      <c r="AF39">
+        <v>1</v>
+      </c>
+      <c r="AG39">
+        <f>(Tabelle5[[#This Row],[Spalte2]]+Tabelle5[[#This Row],[Spalte3]]+Tabelle5[[#This Row],[Spalte4]]+Tabelle5[[#This Row],[Spalte5]])/4</f>
+        <v>1.25</v>
+      </c>
+    </row>
+    <row r="40" spans="8:33" x14ac:dyDescent="0.2">
       <c r="H40" s="3"/>
       <c r="J40" s="1">
         <v>31</v>
@@ -2357,8 +5223,27 @@
       <c r="N40" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="41" spans="8:14" x14ac:dyDescent="0.2">
+      <c r="AB40">
+        <v>33</v>
+      </c>
+      <c r="AC40">
+        <v>3</v>
+      </c>
+      <c r="AD40">
+        <v>3</v>
+      </c>
+      <c r="AE40">
+        <v>3</v>
+      </c>
+      <c r="AF40">
+        <v>2</v>
+      </c>
+      <c r="AG40">
+        <f>(Tabelle5[[#This Row],[Spalte2]]+Tabelle5[[#This Row],[Spalte3]]+Tabelle5[[#This Row],[Spalte4]]+Tabelle5[[#This Row],[Spalte5]])/4</f>
+        <v>2.75</v>
+      </c>
+    </row>
+    <row r="41" spans="8:33" x14ac:dyDescent="0.2">
       <c r="H41" s="4"/>
       <c r="J41">
         <v>32</v>
@@ -2366,8 +5251,27 @@
       <c r="L41" s="1">
         <v>0.02</v>
       </c>
-    </row>
-    <row r="42" spans="8:14" x14ac:dyDescent="0.2">
+      <c r="AB41">
+        <v>34</v>
+      </c>
+      <c r="AC41">
+        <v>8</v>
+      </c>
+      <c r="AD41">
+        <v>8</v>
+      </c>
+      <c r="AE41">
+        <v>9</v>
+      </c>
+      <c r="AF41">
+        <v>9</v>
+      </c>
+      <c r="AG41">
+        <f>(Tabelle5[[#This Row],[Spalte2]]+Tabelle5[[#This Row],[Spalte3]]+Tabelle5[[#This Row],[Spalte4]]+Tabelle5[[#This Row],[Spalte5]])/4</f>
+        <v>8.5</v>
+      </c>
+    </row>
+    <row r="42" spans="8:33" x14ac:dyDescent="0.2">
       <c r="H42" s="3"/>
       <c r="J42">
         <v>33</v>
@@ -2375,8 +5279,27 @@
       <c r="L42" s="1">
         <v>0.02</v>
       </c>
-    </row>
-    <row r="43" spans="8:14" x14ac:dyDescent="0.2">
+      <c r="AB42">
+        <v>35</v>
+      </c>
+      <c r="AC42">
+        <v>13</v>
+      </c>
+      <c r="AD42">
+        <v>14</v>
+      </c>
+      <c r="AE42">
+        <v>14</v>
+      </c>
+      <c r="AF42">
+        <v>14</v>
+      </c>
+      <c r="AG42">
+        <f>(Tabelle5[[#This Row],[Spalte2]]+Tabelle5[[#This Row],[Spalte3]]+Tabelle5[[#This Row],[Spalte4]]+Tabelle5[[#This Row],[Spalte5]])/4</f>
+        <v>13.75</v>
+      </c>
+    </row>
+    <row r="43" spans="8:33" x14ac:dyDescent="0.2">
       <c r="H43" s="4"/>
       <c r="J43">
         <v>34</v>
@@ -2384,8 +5307,27 @@
       <c r="L43" s="1">
         <v>0.1</v>
       </c>
-    </row>
-    <row r="44" spans="8:14" x14ac:dyDescent="0.2">
+      <c r="AB43">
+        <v>36</v>
+      </c>
+      <c r="AC43">
+        <v>19</v>
+      </c>
+      <c r="AD43">
+        <v>20</v>
+      </c>
+      <c r="AE43">
+        <v>20</v>
+      </c>
+      <c r="AF43">
+        <v>19</v>
+      </c>
+      <c r="AG43">
+        <f>(Tabelle5[[#This Row],[Spalte2]]+Tabelle5[[#This Row],[Spalte3]]+Tabelle5[[#This Row],[Spalte4]]+Tabelle5[[#This Row],[Spalte5]])/4</f>
+        <v>19.5</v>
+      </c>
+    </row>
+    <row r="44" spans="8:33" x14ac:dyDescent="0.2">
       <c r="H44" s="3"/>
       <c r="J44">
         <v>35</v>
@@ -2393,8 +5335,27 @@
       <c r="L44" s="1">
         <v>0.19</v>
       </c>
-    </row>
-    <row r="45" spans="8:14" x14ac:dyDescent="0.2">
+      <c r="AB44">
+        <v>37</v>
+      </c>
+      <c r="AC44">
+        <v>18</v>
+      </c>
+      <c r="AD44">
+        <v>19</v>
+      </c>
+      <c r="AE44">
+        <v>19</v>
+      </c>
+      <c r="AF44">
+        <v>19</v>
+      </c>
+      <c r="AG44">
+        <f>(Tabelle5[[#This Row],[Spalte2]]+Tabelle5[[#This Row],[Spalte3]]+Tabelle5[[#This Row],[Spalte4]]+Tabelle5[[#This Row],[Spalte5]])/4</f>
+        <v>18.75</v>
+      </c>
+    </row>
+    <row r="45" spans="8:33" x14ac:dyDescent="0.2">
       <c r="H45" s="4"/>
       <c r="J45">
         <v>36</v>
@@ -2402,8 +5363,27 @@
       <c r="L45" s="1">
         <v>0.32</v>
       </c>
-    </row>
-    <row r="46" spans="8:14" x14ac:dyDescent="0.2">
+      <c r="AB45">
+        <v>38</v>
+      </c>
+      <c r="AC45">
+        <v>12</v>
+      </c>
+      <c r="AD45">
+        <v>14</v>
+      </c>
+      <c r="AE45">
+        <v>13</v>
+      </c>
+      <c r="AF45">
+        <v>15</v>
+      </c>
+      <c r="AG45">
+        <f>(Tabelle5[[#This Row],[Spalte2]]+Tabelle5[[#This Row],[Spalte3]]+Tabelle5[[#This Row],[Spalte4]]+Tabelle5[[#This Row],[Spalte5]])/4</f>
+        <v>13.5</v>
+      </c>
+    </row>
+    <row r="46" spans="8:33" x14ac:dyDescent="0.2">
       <c r="H46" s="3"/>
       <c r="J46">
         <v>37</v>
@@ -2411,8 +5391,27 @@
       <c r="L46" s="1">
         <v>0.39</v>
       </c>
-    </row>
-    <row r="47" spans="8:14" x14ac:dyDescent="0.2">
+      <c r="AB46">
+        <v>39</v>
+      </c>
+      <c r="AC46">
+        <v>7</v>
+      </c>
+      <c r="AD46">
+        <v>8</v>
+      </c>
+      <c r="AE46">
+        <v>8</v>
+      </c>
+      <c r="AF46">
+        <v>9</v>
+      </c>
+      <c r="AG46">
+        <f>(Tabelle5[[#This Row],[Spalte2]]+Tabelle5[[#This Row],[Spalte3]]+Tabelle5[[#This Row],[Spalte4]]+Tabelle5[[#This Row],[Spalte5]])/4</f>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="47" spans="8:33" x14ac:dyDescent="0.2">
       <c r="H47" s="4"/>
       <c r="J47">
         <v>38</v>
@@ -2420,8 +5419,27 @@
       <c r="L47" s="1">
         <v>0.41</v>
       </c>
-    </row>
-    <row r="48" spans="8:14" x14ac:dyDescent="0.2">
+      <c r="AB47">
+        <v>40</v>
+      </c>
+      <c r="AC47">
+        <v>3</v>
+      </c>
+      <c r="AD47">
+        <v>5</v>
+      </c>
+      <c r="AE47">
+        <v>4</v>
+      </c>
+      <c r="AF47">
+        <v>5</v>
+      </c>
+      <c r="AG47">
+        <f>(Tabelle5[[#This Row],[Spalte2]]+Tabelle5[[#This Row],[Spalte3]]+Tabelle5[[#This Row],[Spalte4]]+Tabelle5[[#This Row],[Spalte5]])/4</f>
+        <v>4.25</v>
+      </c>
+    </row>
+    <row r="48" spans="8:33" x14ac:dyDescent="0.2">
       <c r="H48" s="3"/>
       <c r="J48">
         <v>39</v>
@@ -2429,8 +5447,27 @@
       <c r="L48" s="1">
         <v>0.38</v>
       </c>
-    </row>
-    <row r="49" spans="8:12" x14ac:dyDescent="0.2">
+      <c r="AB48">
+        <v>41</v>
+      </c>
+      <c r="AC48">
+        <v>1</v>
+      </c>
+      <c r="AD48">
+        <v>2</v>
+      </c>
+      <c r="AE48">
+        <v>2</v>
+      </c>
+      <c r="AF48">
+        <v>2</v>
+      </c>
+      <c r="AG48">
+        <f>(Tabelle5[[#This Row],[Spalte2]]+Tabelle5[[#This Row],[Spalte3]]+Tabelle5[[#This Row],[Spalte4]]+Tabelle5[[#This Row],[Spalte5]])/4</f>
+        <v>1.75</v>
+      </c>
+    </row>
+    <row r="49" spans="8:33" x14ac:dyDescent="0.2">
       <c r="H49" s="4"/>
       <c r="J49">
         <v>40</v>
@@ -2438,42 +5475,451 @@
       <c r="L49" s="1">
         <v>0.35</v>
       </c>
-    </row>
-    <row r="50" spans="8:12" x14ac:dyDescent="0.2">
+      <c r="AB49">
+        <v>42</v>
+      </c>
+      <c r="AC49">
+        <v>0</v>
+      </c>
+      <c r="AD49">
+        <v>1</v>
+      </c>
+      <c r="AE49">
+        <v>1</v>
+      </c>
+      <c r="AF49">
+        <v>1</v>
+      </c>
+      <c r="AG49">
+        <f>(Tabelle5[[#This Row],[Spalte2]]+Tabelle5[[#This Row],[Spalte3]]+Tabelle5[[#This Row],[Spalte4]]+Tabelle5[[#This Row],[Spalte5]])/4</f>
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="50" spans="8:33" x14ac:dyDescent="0.2">
       <c r="H50" s="3"/>
       <c r="J50">
         <v>41</v>
       </c>
-    </row>
-    <row r="51" spans="8:12" x14ac:dyDescent="0.2">
+      <c r="AB50">
+        <v>43</v>
+      </c>
+      <c r="AC50">
+        <v>0</v>
+      </c>
+      <c r="AD50">
+        <v>0</v>
+      </c>
+      <c r="AE50">
+        <v>0</v>
+      </c>
+      <c r="AF50">
+        <v>0</v>
+      </c>
+      <c r="AG50">
+        <f>(Tabelle5[[#This Row],[Spalte2]]+Tabelle5[[#This Row],[Spalte3]]+Tabelle5[[#This Row],[Spalte4]]+Tabelle5[[#This Row],[Spalte5]])/4</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="8:33" x14ac:dyDescent="0.2">
       <c r="J51">
         <v>42</v>
       </c>
-    </row>
-    <row r="52" spans="8:12" x14ac:dyDescent="0.2">
+      <c r="AB51">
+        <v>44</v>
+      </c>
+      <c r="AC51">
+        <v>0</v>
+      </c>
+      <c r="AD51">
+        <v>0</v>
+      </c>
+      <c r="AE51">
+        <v>0</v>
+      </c>
+      <c r="AF51">
+        <v>0</v>
+      </c>
+      <c r="AG51">
+        <f>(Tabelle5[[#This Row],[Spalte2]]+Tabelle5[[#This Row],[Spalte3]]+Tabelle5[[#This Row],[Spalte4]]+Tabelle5[[#This Row],[Spalte5]])/4</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="8:33" x14ac:dyDescent="0.2">
       <c r="J52">
         <v>43</v>
       </c>
-    </row>
-    <row r="53" spans="8:12" x14ac:dyDescent="0.2">
+      <c r="AB52">
+        <v>45</v>
+      </c>
+      <c r="AC52">
+        <v>1</v>
+      </c>
+      <c r="AD52">
+        <v>0</v>
+      </c>
+      <c r="AE52">
+        <v>0</v>
+      </c>
+      <c r="AF52">
+        <v>0</v>
+      </c>
+      <c r="AG52">
+        <f>(Tabelle5[[#This Row],[Spalte2]]+Tabelle5[[#This Row],[Spalte3]]+Tabelle5[[#This Row],[Spalte4]]+Tabelle5[[#This Row],[Spalte5]])/4</f>
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="53" spans="8:33" x14ac:dyDescent="0.2">
       <c r="J53">
         <v>44</v>
       </c>
-    </row>
-    <row r="54" spans="8:12" x14ac:dyDescent="0.2">
+      <c r="AB53">
+        <v>46</v>
+      </c>
+      <c r="AC53">
+        <v>2</v>
+      </c>
+      <c r="AD53">
+        <v>1</v>
+      </c>
+      <c r="AE53">
+        <v>1</v>
+      </c>
+      <c r="AF53">
+        <v>1</v>
+      </c>
+      <c r="AG53">
+        <f>(Tabelle5[[#This Row],[Spalte2]]+Tabelle5[[#This Row],[Spalte3]]+Tabelle5[[#This Row],[Spalte4]]+Tabelle5[[#This Row],[Spalte5]])/4</f>
+        <v>1.25</v>
+      </c>
+    </row>
+    <row r="54" spans="8:33" x14ac:dyDescent="0.2">
       <c r="J54">
         <v>45</v>
+      </c>
+      <c r="AB54">
+        <v>47</v>
+      </c>
+      <c r="AC54">
+        <v>5</v>
+      </c>
+      <c r="AD54">
+        <v>4</v>
+      </c>
+      <c r="AE54">
+        <v>5</v>
+      </c>
+      <c r="AF54">
+        <v>4</v>
+      </c>
+      <c r="AG54">
+        <f>(Tabelle5[[#This Row],[Spalte2]]+Tabelle5[[#This Row],[Spalte3]]+Tabelle5[[#This Row],[Spalte4]]+Tabelle5[[#This Row],[Spalte5]])/4</f>
+        <v>4.5</v>
+      </c>
+    </row>
+    <row r="55" spans="8:33" x14ac:dyDescent="0.2">
+      <c r="AB55">
+        <v>48</v>
+      </c>
+      <c r="AC55">
+        <v>10</v>
+      </c>
+      <c r="AD55">
+        <v>9</v>
+      </c>
+      <c r="AE55">
+        <v>9</v>
+      </c>
+      <c r="AF55">
+        <v>9</v>
+      </c>
+      <c r="AG55">
+        <f>(Tabelle5[[#This Row],[Spalte2]]+Tabelle5[[#This Row],[Spalte3]]+Tabelle5[[#This Row],[Spalte4]]+Tabelle5[[#This Row],[Spalte5]])/4</f>
+        <v>9.25</v>
+      </c>
+    </row>
+    <row r="56" spans="8:33" x14ac:dyDescent="0.2">
+      <c r="AB56">
+        <v>49</v>
+      </c>
+      <c r="AC56">
+        <v>19</v>
+      </c>
+      <c r="AD56">
+        <v>16</v>
+      </c>
+      <c r="AE56">
+        <v>16</v>
+      </c>
+      <c r="AF56">
+        <v>15</v>
+      </c>
+      <c r="AG56">
+        <f>(Tabelle5[[#This Row],[Spalte2]]+Tabelle5[[#This Row],[Spalte3]]+Tabelle5[[#This Row],[Spalte4]]+Tabelle5[[#This Row],[Spalte5]])/4</f>
+        <v>16.5</v>
+      </c>
+    </row>
+    <row r="57" spans="8:33" x14ac:dyDescent="0.2">
+      <c r="AB57">
+        <v>50</v>
+      </c>
+      <c r="AC57">
+        <v>21</v>
+      </c>
+      <c r="AD57">
+        <v>21</v>
+      </c>
+      <c r="AE57">
+        <v>20</v>
+      </c>
+      <c r="AF57">
+        <v>21</v>
+      </c>
+      <c r="AG57">
+        <f>(Tabelle5[[#This Row],[Spalte2]]+Tabelle5[[#This Row],[Spalte3]]+Tabelle5[[#This Row],[Spalte4]]+Tabelle5[[#This Row],[Spalte5]])/4</f>
+        <v>20.75</v>
+      </c>
+    </row>
+    <row r="58" spans="8:33" x14ac:dyDescent="0.2">
+      <c r="AB58">
+        <v>51</v>
+      </c>
+      <c r="AC58">
+        <v>21</v>
+      </c>
+      <c r="AD58">
+        <v>21</v>
+      </c>
+      <c r="AE58">
+        <v>20</v>
+      </c>
+      <c r="AF58">
+        <v>19</v>
+      </c>
+      <c r="AG58">
+        <f>(Tabelle5[[#This Row],[Spalte2]]+Tabelle5[[#This Row],[Spalte3]]+Tabelle5[[#This Row],[Spalte4]]+Tabelle5[[#This Row],[Spalte5]])/4</f>
+        <v>20.25</v>
+      </c>
+    </row>
+    <row r="59" spans="8:33" x14ac:dyDescent="0.2">
+      <c r="AB59">
+        <v>52</v>
+      </c>
+      <c r="AC59">
+        <v>15</v>
+      </c>
+      <c r="AD59">
+        <v>18</v>
+      </c>
+      <c r="AE59">
+        <v>16</v>
+      </c>
+      <c r="AF59">
+        <v>15</v>
+      </c>
+      <c r="AG59">
+        <f>(Tabelle5[[#This Row],[Spalte2]]+Tabelle5[[#This Row],[Spalte3]]+Tabelle5[[#This Row],[Spalte4]]+Tabelle5[[#This Row],[Spalte5]])/4</f>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="60" spans="8:33" x14ac:dyDescent="0.2">
+      <c r="AB60">
+        <v>53</v>
+      </c>
+      <c r="AC60">
+        <v>9</v>
+      </c>
+      <c r="AD60">
+        <v>12</v>
+      </c>
+      <c r="AE60">
+        <v>12</v>
+      </c>
+      <c r="AF60">
+        <v>10</v>
+      </c>
+      <c r="AG60">
+        <f>(Tabelle5[[#This Row],[Spalte2]]+Tabelle5[[#This Row],[Spalte3]]+Tabelle5[[#This Row],[Spalte4]]+Tabelle5[[#This Row],[Spalte5]])/4</f>
+        <v>10.75</v>
+      </c>
+    </row>
+    <row r="61" spans="8:33" x14ac:dyDescent="0.2">
+      <c r="AB61">
+        <v>54</v>
+      </c>
+      <c r="AC61">
+        <v>4</v>
+      </c>
+      <c r="AD61">
+        <v>7</v>
+      </c>
+      <c r="AE61">
+        <v>6</v>
+      </c>
+      <c r="AF61">
+        <v>7</v>
+      </c>
+      <c r="AG61">
+        <f>(Tabelle5[[#This Row],[Spalte2]]+Tabelle5[[#This Row],[Spalte3]]+Tabelle5[[#This Row],[Spalte4]]+Tabelle5[[#This Row],[Spalte5]])/4</f>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="62" spans="8:33" x14ac:dyDescent="0.2">
+      <c r="AB62">
+        <v>55</v>
+      </c>
+      <c r="AC62">
+        <v>2</v>
+      </c>
+      <c r="AD62">
+        <v>3</v>
+      </c>
+      <c r="AE62">
+        <v>2</v>
+      </c>
+      <c r="AF62">
+        <v>4</v>
+      </c>
+      <c r="AG62">
+        <f>(Tabelle5[[#This Row],[Spalte2]]+Tabelle5[[#This Row],[Spalte3]]+Tabelle5[[#This Row],[Spalte4]]+Tabelle5[[#This Row],[Spalte5]])/4</f>
+        <v>2.75</v>
+      </c>
+    </row>
+    <row r="63" spans="8:33" x14ac:dyDescent="0.2">
+      <c r="AB63">
+        <v>56</v>
+      </c>
+      <c r="AC63">
+        <v>1</v>
+      </c>
+      <c r="AD63">
+        <v>1</v>
+      </c>
+      <c r="AE63">
+        <v>1</v>
+      </c>
+      <c r="AF63">
+        <v>1</v>
+      </c>
+      <c r="AG63">
+        <f>(Tabelle5[[#This Row],[Spalte2]]+Tabelle5[[#This Row],[Spalte3]]+Tabelle5[[#This Row],[Spalte4]]+Tabelle5[[#This Row],[Spalte5]])/4</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="64" spans="8:33" x14ac:dyDescent="0.2">
+      <c r="AB64">
+        <v>57</v>
+      </c>
+      <c r="AC64">
+        <v>0</v>
+      </c>
+      <c r="AD64">
+        <v>0</v>
+      </c>
+      <c r="AE64">
+        <v>0</v>
+      </c>
+      <c r="AF64">
+        <v>0</v>
+      </c>
+      <c r="AG64">
+        <f>(Tabelle5[[#This Row],[Spalte2]]+Tabelle5[[#This Row],[Spalte3]]+Tabelle5[[#This Row],[Spalte4]]+Tabelle5[[#This Row],[Spalte5]])/4</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="65" spans="28:33" x14ac:dyDescent="0.2">
+      <c r="AB65">
+        <v>58</v>
+      </c>
+      <c r="AC65">
+        <v>0</v>
+      </c>
+      <c r="AD65">
+        <v>0</v>
+      </c>
+      <c r="AE65">
+        <v>0</v>
+      </c>
+      <c r="AF65">
+        <v>0</v>
+      </c>
+      <c r="AG65">
+        <f>(Tabelle5[[#This Row],[Spalte2]]+Tabelle5[[#This Row],[Spalte3]]+Tabelle5[[#This Row],[Spalte4]]+Tabelle5[[#This Row],[Spalte5]])/4</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="66" spans="28:33" x14ac:dyDescent="0.2">
+      <c r="AB66">
+        <v>59</v>
+      </c>
+      <c r="AC66">
+        <v>1</v>
+      </c>
+      <c r="AD66">
+        <v>1</v>
+      </c>
+      <c r="AE66">
+        <v>0</v>
+      </c>
+      <c r="AF66">
+        <v>0</v>
+      </c>
+      <c r="AG66">
+        <f>(Tabelle5[[#This Row],[Spalte2]]+Tabelle5[[#This Row],[Spalte3]]+Tabelle5[[#This Row],[Spalte4]]+Tabelle5[[#This Row],[Spalte5]])/4</f>
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="67" spans="28:33" x14ac:dyDescent="0.2">
+      <c r="AB67">
+        <v>60</v>
+      </c>
+      <c r="AC67">
+        <v>2</v>
+      </c>
+      <c r="AD67">
+        <v>3</v>
+      </c>
+      <c r="AE67">
+        <v>2</v>
+      </c>
+      <c r="AF67">
+        <v>1</v>
+      </c>
+      <c r="AG67">
+        <f>(Tabelle5[[#This Row],[Spalte2]]+Tabelle5[[#This Row],[Spalte3]]+Tabelle5[[#This Row],[Spalte4]]+Tabelle5[[#This Row],[Spalte5]])/4</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="68" spans="28:33" x14ac:dyDescent="0.2">
+      <c r="AB68">
+        <v>61</v>
+      </c>
+      <c r="AC68">
+        <v>5</v>
+      </c>
+      <c r="AD68">
+        <v>6</v>
+      </c>
+      <c r="AE68">
+        <v>5</v>
+      </c>
+      <c r="AF68">
+        <v>3</v>
+      </c>
+      <c r="AG68">
+        <f>(Tabelle5[[#This Row],[Spalte2]]+Tabelle5[[#This Row],[Spalte3]]+Tabelle5[[#This Row],[Spalte4]]+Tabelle5[[#This Row],[Spalte5]])/4</f>
+        <v>4.75</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
-  <tableParts count="4">
+  <tableParts count="5">
     <tablePart r:id="rId2"/>
     <tablePart r:id="rId3"/>
     <tablePart r:id="rId4"/>
     <tablePart r:id="rId5"/>
+    <tablePart r:id="rId6"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>